<commit_message>
add contact to excel
</commit_message>
<xml_diff>
--- a/divar.xlsx
+++ b/divar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,11 @@
           <t>sub_type</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>contact</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -526,7 +531,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>زمین‌ 400 مترمربع سنددار</t>
+          <t>آپارتمان ۵۰متر و ۷۰دسیمتر حدادعادل</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -536,34 +541,61 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>اندیشه</t>
+          <t>کوثر</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/زمین-400-مترمربع-سنددار_زمین-و-کلنگی_تهران_اندیشه_دیوار/gY923DeO</t>
+          <t>https://divar.ir/v/آپارتمان-۵۰متر-و-۷۰دسیمتر-حدادعادل_آپارتمان_تهران_کوثر_دیوار/gY6K8AgW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>زمینی بامتراژ 400 مترمربع،
-سنددار،
-مجموعه 17 هکتاری،
-اقامتی و تفریحی،
-اولین جزیره ی سندداردرایران،
-اقامت رایگان درصورت خرید</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+          <t>تا اول ابان مستاجر دارد.
+درب و دستگیره سرویس ها تازه تعویض شده.
+سند تک برگ.
+۲کمددیواری بزرگ.
+آیفون تصویری.
+کوچه ماشین رو.
+جای پارک موتور دارد و درصورت اجازه همسایه ها امکان استفاده دارد.
+قیمت مقطوع.املاکی های محترم قیمت مقطوع مقطوع میباشد.زیرا مبلغی که برای تخفیف درنظر گرفته بودیم برای تعویض دربها هزینه شد. لطفا برای چانه زدن و کاهش قیمت تماس نگیرید و وقت خود و ما را نگیرید.
+عکسهای بارگذاری شده مربوط به قبل از تعویض دربها میباشد.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>۱۳۷۹</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>۵۰</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>قیمت هر متر۲٬۵۰۰٬۰۰۰ تومان</t>
+          <t>قیمت هر متر۲۰٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -583,7 +615,12 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>زمین و کلنگی</t>
+          <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>09374258056</t>
         </is>
       </c>
     </row>
@@ -593,81 +630,47 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ویلایی 120متر زمین  هر طبقه ۷۵ متر بنا میعاد شمالی</t>
+          <t>باغ باغچه شهریار یوسف آباد صیرفی</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>۸,۲۵۰,۰۰۰,۰۰۰ تومان</t>
+          <t>توافقی</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>نو</t>
+          <t>تهران‌سر</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/ویلایی-120متر-زمین-هر-طبقه-۷۵-متر-بنا-میعاد-شمالی_خانه-و-ویلا_تهران_خانی-آباد-نو_دیوار/gYLaQ90c</t>
+          <t>https://divar.ir/v/باغ-باغچه-شهریار-یوسف-آباد-صیرفی_زمین-و-کلنگی_تهران_تهران-سر_دیوار/gY1qfX3L</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>سلام 
-قابل توجه ی مشاور املاک های عزیز بابت فایل کردن و همکاری 
-قیمت نسبت به سال ساخت و استحکام ساختمان نسبتا بالاست خواهشن با ملک کلنگی ۵۰ سال مقایسه نکنید
- ی مقدار هزینه کنید عالی میشه
- برای مصرف کننده پر جمعیت و شخصی خوبه 
-اسکلت و استخون بندی ساختمان عالی 
-ملک فوق شخصی ساز سال ساخت و جواز ساخت ۱۳۸۱ 
-سازه تمام اسکلت سقفها سفال بتنی با فندانسیون عالی و اسکلت تیر آهن ۱۸ دوبل 
-ملک قابل سکونت بوده در حال حاضر خودمان ساکن هستیم .
-طبقه اول پارکینگ بوده که مسکونی شده سقف کوتاه و کمی هزینه داره
-طبقه دوم و سوم سرویس کامل و تمیز 
-هرطبقه متراژ ۷۵ متر 
-یک خواب ۱۵ متر ی
-اشپزخانه ۱۵ متر کابینت ممبران ترک اجاق گاز رو میزی
-سیستم گرمایش و اب گرم پکیج میباشد 
-سه خط تلفن 
-سه تا کنتور برق
-گاز و آب مشترک
-۲۰ متر نشیمن ۲۰ متر پذیرایی سرویس حمام ۳ متر و سرویس دستشویی ۲متر 
-حیاط ۲۰ متر جای پارک یک ماشین 
-فروش بصورت کلیدی و سند مادر دارد طبقات تفکیک نشده
- فقط ملک یک سند مادر منگوله دار  دارد  
-ملک پایانکار ندارد بعلت خلافی داخل ساختمان و مسکونی کردن پارکینگ  
-مناسب خانواده های پر جمعیت و شخصی</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>۱۳۸۱</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>۱</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>۱۵۰</t>
-        </is>
-      </c>
+          <t>با سلام /شهرک باغ برای تعاونی مسکن کارکنان شهرداری 
+در شهریار یوسف آباد صیرفی موقعیت جغرافیایی. 1سال اقساطی در بانک 
+یکی از تعاونی های خوشنام وبا سابقه و رزومه درخشان در زمینی به مساحت 20هکتاری مناطقه خوش آب و هوا شهریار 
+500متری و 1000متری نموده است 
+باغچه دارای سند و دفتر چه آب برق
+توضیح بیشتر تماس بگیرید</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>انباری ندارد</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>قیمت کلتوافقی</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr">
         <is>
           <t>sell</t>
@@ -680,7 +683,12 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>خانه و ویلا</t>
+          <t>زمین و کلنگی</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>09123143251</t>
         </is>
       </c>
     </row>
@@ -690,65 +698,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>اپارتمان ۵۸ متری مشیریه</t>
+          <t>سوییت آپارتمان فول امکانات صادقیه</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ودیعه: ۲۵۰,۰۰۰,۰۰۰ تومان
-اجاره ماهیانه: ۱۰۰,۰۰۰ تومان</t>
+          <t>اجاره روزانه: ۴۹۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>مشیریه</t>
+          <t>صادقیه</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اپارتمان-۵۸-متری-مشیریه_آپارتمان_تهران_مشیریه_دیوار/gY9yHMVA</t>
+          <t>https://divar.ir/v/سوییت-آپارتمان-فول-امکانات-صادقیه_آپارتمان-و-سوئیت_تهران_صادقیه_دیوار/gY9aGSPr</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>طبقه اول تک واحدی حیاط خلوت مسقف</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>۱۳۸۲</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>۱</t>
-        </is>
-      </c>
+          <t>واحد 110 متری
+دسترسی به مترو صادقیه و BRT
+۱ خواب
+با پارکینگ و اسانسور ( مجهز ب دوربین )
+سیستم صوتی مناسب
+سرویس ایرانی فرنگی
+امنیت بالا محیطی ارام
+نگهبانی 
+سیستم گرمایشی پکیج 
+لوازم پخت و پز
+امکانات رفاهی کامل برای اقامتی راحت
+** نظافت و ضدعفونی کامل بعد از هربار خروج مهمان قبل **
+((بارعایت پروتکل های بهداشتی))
+برای هماهنگی و رزرو فقط تماس بگیرید
+فقط در صورت مشغول بودن پیامک دهید</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>۵۸</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>طبقه۱</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>پارکینگ ندارد</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>آسانسور ندارد</t>
-        </is>
-      </c>
+          <t>۱۰۰</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
@@ -758,12 +755,17 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>اجاره کوتاه مدت</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>آپارتمان و سوئیت</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>09961912709</t>
         </is>
       </c>
     </row>
@@ -773,69 +775,51 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>۵۰ متر یه خوابه کارون</t>
+          <t>مغازه ۱۳ متری</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ودیعه: ۲۵۰,۰۰۰,۰۰۰ تومان
-اجاره ماهیانه: مجانی</t>
+          <t>ودیعه: ۱۵۰,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: ۵,۱۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>جیحون</t>
+          <t>مرکزی</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/۵۰-متر-یه-خوابه-کارون_آپارتمان_تهران_جیحون_دیوار/gY9uXOqJ</t>
+          <t>https://divar.ir/v/مغازه-۱۳-متری_مغازه-و-غرفه_تهران_جنت-آباد-مرکزی_دیوار/gY9GJVSa</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>واحد فوق به صورت رهن کامل اجاره داده می‌شود
-بدون مالک
-دسترسی راحت
-آماده تخلیه
-بازدید تمام وقت</t>
+          <t>پاساژ طوبی جنت آباد مرکزی 
+کف سنگ 
+بحر ۳
+آب برق تلفن
+نگهبانی ۲۴ ساعته
+سرمایش و گرمایش 
+مناسب جهت انواع صنوف</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>۱۳۸۲</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>۱</t>
-        </is>
-      </c>
+          <t>۱۳۸۵</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>۵۰</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>طبقه۱</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>پارکینگ ندارد</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>آسانسور ندارد</t>
-        </is>
-      </c>
+          <t>۱۳</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
@@ -845,12 +829,17 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>اجاره اداری و تجاری</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>مغازه و غرفه</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>09909673775</t>
         </is>
       </c>
     </row>
@@ -860,68 +849,86 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3 هکتار دیوار کشی  پایان کار دار</t>
+          <t>اپارتمان ۵۵ متری تک خواب</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>۳۳,۰۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۲۷۵,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: مجانی</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>تهران‌سر</t>
+          <t>جنوبی</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/3-هکتار-دیوار-کشی-پایان-کار-دار_صنعتی-کشاورزی-و-تجاری_تهران_تهران-سر_دیوار/gY92nLIw</t>
+          <t>https://divar.ir/v/اپارتمان-۵۵-متری-تک-خواب_آپارتمان_تهران_نارمک-جنوبی_دیوار/gY9GpuUx</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3  هکتار  مین 4  دیواری موقعیت  عالی  
-دارای  برق 3  فاز
-1  برق  تک فاز 
-چاه آب 
-حق آباه 
-موقعیت  سرمایه گذاری  عالی  کریدور  اصلی</t>
+          <t>رهن کامل.
+ملک تخلیه میباشد</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>۱۴۰۰</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۱٬۱۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>قیمت کل۳۳٬۰۰۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+          <t>۱۳۸۰</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>۵۵</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>طبقه۱ از ۴</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>فروش اداری و تجاری</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>صنعتی، کشاورزی و تجاری</t>
+          <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>09105825579</t>
         </is>
       </c>
     </row>
@@ -931,72 +938,43 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>آپارتمان ۱۱۷ متری ۳ خوابه با ۲ پارکینگ سندی</t>
+          <t>۱۰۴ متری پروژه نارنجستان ۴</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>۶,۳۸۰,۰۰۰,۰۰۰ تومان</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>دهقان</t>
+          <t>فارس</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۱۱۷-متری-۳-خوابه-با-۲-پارکینگ-سندی_آپارتمان_تهران_دهقان_دیوار/gY9uXrMA</t>
+          <t>https://divar.ir/v/۱۰۴-متری-پروژه-نارنجستان-۴_پیش-فروش_تهران_دریاچه-شهدای-خلیج-فارس_دیوار/gY9KJQbM</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>۱۱۷ متر نوساز فول امکانات. متریال برند. خیابان اول نیروهوایی
-دارای ۲ پارکینگ سندی غیر مزاحم و انباری
-تحویل شهریور ماه</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>۱۴۰۰</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>۳</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>۱۱۷</t>
-        </is>
-      </c>
+          <t>تیپ ۱۰۴ متری نارنجستان ۴
+واریزی ۸۴۳
+امتیاز ۹۷۰
+رتبه تک رقمی
+فقط پیام پاسخگو هستم
+املاک در صورت داشتن مشتری تماس بگیرن</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۵۴٬۵۲۹٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>قیمت کل۶٬۳۸۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
           <t>sell</t>
@@ -1004,12 +982,17 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>پرو‌ژه‌های ساخت و ساز</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>پیش‌فروش</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>09105213447</t>
         </is>
       </c>
     </row>
@@ -1019,64 +1002,88 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>آپارتمان مبله  ۱۳۰m سه خواب میرداماد بیواسطه</t>
+          <t>آپارتمان 88 متر نوساز غرق در نور  (جی)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>اجاره روزانه: ۱,۵۰۰,۰۰۰ تومان</t>
+          <t>۲,۵۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>میرداماد</t>
+          <t>جی</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-مبله-۱۳۰m-سه-خواب-میرداماد-بیواسطه_آپارتمان-و-سوئیت_تهران_میرداماد_دیوار/QY1llN9T</t>
+          <t>https://divar.ir/v/آپارتمان-88-متر-نوساز-غرق-در-نور-جی-_آپارتمان_تهران_جی_دیوار/gY9KZppX</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>اجاره آپارتمان مبله شیک و لوکس با تمام امکانات رفاهی با  آسانسور و پارکینگ 
-سرایداری مقیم  
-ویو و چشم انداز عالی 
-دسترسی عالی به مراکز خرید مترو شریعتی و مراکز درمانی 
-مدیریت واحدبا ضد عفونی و
-شستشوی کلیه ملحفه و روبالشی ها بصورت هرروز سعی در کنترل و ایمن نگاه داشتن مهمانان از ویروس کرونا را دارند.
-واحد طبقه همکف ،آخر هفته ها ۲۰درصد افزایش قیمت داریم.
-جهت رزرو ساعت تماس ۱۱ الی ۱بامداد
-مهندس نظامدوست
-۰۹۱۲۴۴۴۶۴۴۸</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+          <t>آپارتمان نوساز غرق در نور پذیرایی پرده خور و هر 2خواب نور گیر عالی. حدودا 9متر پاسیو(حیاط خلوت) مسقف. کابینت، های گلاس. دارای بالکن. واحد های هرطبقه جدا (شرقی و غربی).</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>۱۴۰۰</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>۲</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>۱۳۰</t>
+          <t>۸۸</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>آسانسور</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۲۸٬۴۰۹٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>قیمت کل۲٬۵۰۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>اجاره کوتاه مدت</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>آپارتمان و سوئیت</t>
+          <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>09104544881</t>
         </is>
       </c>
     </row>
@@ -1086,45 +1093,41 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>آپارتمان دو خواب فول امکانات</t>
+          <t>اجاره آپارتمان ۸۵ متری یک خوابه</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ودیعه: ۵۵۰,۰۰۰,۰۰۰ تومان
-اجاره ماهیانه: مجانی</t>
+          <t>ودیعه: ۱۰۰,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: ۴,۷۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>سهروردی</t>
+          <t>افسریه</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-دو-خواب-فول-امکانات_آپارتمان_تهران_سهروردی_دیوار/gY6auqtS</t>
+          <t>https://divar.ir/v/اجاره-آپارتمان-۸۵-متری-یک-خوابه_خانه-و-ویلا_تهران_افسریه_دیوار/gY9K5w2J</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>آپارتمان دو خواب
-محدوده خیابان مطهری نزدیک مترو مفتح
-فول امکانات
-۸۵ متر 
-نورگیر عالی
-دسترسی راحت به اتوبان، مترو ، بی آر تی و مراکز خرید 
-  **کابینت و کاغذ دیواری ها کهنه میباشد در صورت بازسازی توسط خودتان از مبلغ رهن کسر میشود تا سقف ۳۰ میلیون تومان**
-(( آگهی شخصی میباشد، لطفا املاک تماس نگیرد ))</t>
+          <t>خانه جنوبی طبقه دوم (کلا دو طبقه)
+نورگیر عالی، بازسازی شده، کف کامل موکت، اجاره فقط به دو نفر 
+۰۲۱_۳۳۱۴۹۴۱۸
+۰۹۱۹_۹۱۹۲۴۴۱</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>۱۳۹۱</t>
+          <t>۱۳۷۲</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1132,11 +1135,7 @@
           <t>۸۵</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>طبقه۲</t>
-        </is>
-      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -1147,11 +1146,7 @@
           <t>پارکینگ ندارد</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
@@ -1166,7 +1161,12 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>خانه و ویلا</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>09199192441</t>
         </is>
       </c>
     </row>
@@ -1176,40 +1176,75 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>مغازه زیرپله ۹ متر</t>
+          <t>انبار ۱۵ متری کانتینری مسقف لوازم منزل( غرب تهران</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ودیعه: ۶۰,۰۰۰,۰۰۰ تومان
-اجاره ماهیانه: ۳,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: توافقی
+اجاره ماهیانه: توافقی</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>حسین(ع)</t>
+          <t>تهران‌سر</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/مغازه-زیرپله-۹-متر_مغازه-و-غرفه_تهران_امام-حسین-ع-_دیوار/gY9un5SU</t>
+          <t>https://divar.ir/v/انبار-۱۵-متری-کانتینری-مسقف-لوازم-منزل-غرب-تهران_دفتر-کار-اتاق-اداری-و-مطب_تهران_تهران-سر_دیوار/QX4HnRsh</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>مغازه زیر پله ۹ متر
- گذر عالی و پرتردد دارای کرکره برقی و خط تلفن
-واقع در میدان امام حسین کوچه اسلامی 
-هماهنگی از طریق تماس،</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+          <t>اجاره انبار ۱۵ متری باظرفیت یک کامیون خاور و یک نیسان  وسایل منزل و کالای تجاری داخل کانتینر مسقف و انبار ۳۰ متری باظرفیت سه کامیون خاور  اسباب و اثاثیه
+اجاره انبار اختصاصی بصورت ، ماهانه، سالانه
+بهترین و با کیفیت ترین انبارهای اختصاصی  در جنوب غرب تهران با دسترسی عالی ازتمام نقاط شمال و غرب تهران
+داری مجوز رسمی انبارداری
+دارای امنیت بسیار بالا
+نگهبانان شبانه روزی
+دوربین های مدار بسته دید در شب
+قرارداد رسمی با بیمه
+قفل اختصاصی ( کلید در دست مشتری)
+انبار اختصاصی کانتینری 
+بهترین روش برای نگهداری اسباب و اثاثیه و لوازم منزل و کالای تجاری انبارهای اختصاصی کانتینری می باشد.
+بازدید ۹ صبح الی ۴ عصر
+تلفن انبار: ۴۴۵۸۸۹۱۵
+تلفن همراه : ۰۹۱۲۳۰۸۰۰۴۰
+ارسال لوکیشن و آدرس جهت بازدید و رزروانبار</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>۱۳۹۸</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>۱۵</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>انباری</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
@@ -1224,7 +1259,12 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>مغازه و غرفه</t>
+          <t>دفتر کار، اتاق اداری و مطب</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>09123080040</t>
         </is>
       </c>
     </row>
@@ -1234,47 +1274,54 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>فلکه اول تهرانپارس</t>
+          <t>نارمک ۱۷۰ متری</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>توافقی</t>
+          <t>ودیعه: ۱,۱۰۰,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: مجانی</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>غربی</t>
+          <t>نارمک</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/فلکه-اول-تهرانپارس_آپارتمان_تهران_تهرانپارس-غربی_دیوار/gYxutT89</t>
+          <t>https://divar.ir/v/نارمک-۱۷۰-متری_آپارتمان_تهران_نارمک_دیوار/gY9GZeyd</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>بهترین موقعیت سرمایه گذاری-بدون واسطه
-بدون کوچکترین فضای پرتی
-کابینت ممبران دیوار آینه دکوراتیو کاغذ دیواری برند طراحی داخلی با چوب ترمو کف سنگ حمام مستر کمک دیواری شرایط ایده آل</t>
+          <t>۱۷۰ متر
+دو خواب
+بازسازی
+خیابان رضوان
+حیاط مستقل</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>۱۳۸۸</t>
+          <t>۱۳۷۵</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>۱</t>
+          <t>۲</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>۵۷</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
+          <t>۱۷۰</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>طبقههمکف از ۳</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -1282,33 +1329,34 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>پارکینگ</t>
+          <t>پارکینگ ندارد</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>آسانسور</t>
+          <t>آسانسور ندارد</t>
         </is>
       </c>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>قیمت کلتوافقی</t>
-        </is>
-      </c>
+      <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>09393080055</t>
         </is>
       </c>
     </row>
@@ -1318,7 +1366,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>سعادت آباد،کوهستان،۱۲۷متر،۳خواب</t>
+          <t>رستوران۶۱۲مترمربع. تعویض باملک وخودرو</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1328,52 +1376,38 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>سعادت‌آباد</t>
+          <t>ارم</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/سعادت-آباد-کوهستان-۱۲۷متر-۳خواب_آپارتمان_تهران_سعادت-آباد_دیوار/gYkeGIZ8</t>
+          <t>https://divar.ir/v/رستوران۶۱۲مترمربع-تعویض-باملک-وخودرو_مغازه-و-غرفه_تهران_ارم_دیوار/gY9KJuIf</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>تکواحدی،بر نبش،بالای ۵۰م قدرالسهم ،۲۶ متر سویت-۱
-فقط و فقط در صورت داشتن مشتری املاک ومشاورین محترم تماس بگیرند خواهشا"!!!! لطفا تقاضای عکس نفرمائید،
-بسیار ممنونم...</t>
+          <t>شماره تماس ۰۹۱۹۸۷۳۹۵۱۹و۰۹۱۰۵۸۵۹۶۹۳</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>۱۳۷۹</t>
+          <t>۱۳۸۱</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>۳</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>۱۲۷</t>
+          <t>۶۱۲</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
@@ -1387,12 +1421,17 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>فروش اداری و تجاری</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>مغازه و غرفه</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>09100538975</t>
         </is>
       </c>
     </row>
@@ -1402,70 +1441,66 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>اجاره کارگاه ام دی اف با وسایل</t>
+          <t>اپارتمان ۱۴۰ متر تک واحدی دوخوابه با پاسیو</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ودیعه: توافقی
-اجاره ماهیانه: توافقی</t>
+          <t>ودیعه: ۲۰۰,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: ۱۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ولیعصر</t>
+          <t>پرستار</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اجاره-کارگاه-ام-دی-اف-با-وسایل_صنعتی-کشاورزی-و-تجاری_تهران_شهرک-ولیعصر_دیوار/gY923DcI</t>
+          <t>https://divar.ir/v/اپارتمان-۱۴۰-متر-تک-واحدی-دوخوابه-با-پاسیو_آپارتمان_تهران_پرستار_دیوار/gY9G5bZU</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>با سلام خدمت شما
-اجاره سوله با وسایل ام دی اف
-{مشخصات سوله}
-&gt;سال ساخت ۱۴۰۰
-&gt;متراژ سوله ۲۵۰متر کشیده میباشد
-&gt;دو عدد درب کرکره برقی
-&gt;سرویس بهداشتی
-&gt;روشنایی عالی
-&gt;برق کشی و لوله کشی باد انجام شده
-{مشخصات وسایل کارگاه}
-&gt;دستگاه پی وی سی kdt۳۶۵
-&gt;دستگاه برش ۳۸۰نوین چوب
-&gt;مکنده دو قلو و پمپ باد بزرگ آلمانی
-&gt;دستگاه وکیوم با پمپ ۱۵۰سه ماهه خریداری شده
-&gt;۶عدد میز کار و دستگاه شیار زن
-&gt;اتاق چسب و سنباده برای وکیوم با جنس فلز
-&gt;قفسه نوار پی وی سی و رگال وکیوم
-&gt;دریل۳،اسکا۲،منگنه کوب۲،سنگ فرز۱
-&gt;کولر ۸هزار سپهر یک هفته خریدم
-&gt;گاز ۵شعله،یخچال،تانکر آب،کپسول و...
-&gt;مواد اولیه هم دارم اگه خواستین
-واقع در بر خیابان عرفان آزادگان
-این کارگاه هم مشتری خدمات داره هم میتونین کارهای خودمو بزنین
-من ماهی ۳۰۰میلیون خرید دارم
-فقط پیام جوابگو هستم
-با تشکر از دیوار</t>
+          <t>اپارتمان ۱۴۰ متری دو خوابه دارای دو سرویس بهداشتی مجاز فرنگی و ایرانی بدون دید به سالن 
+دارای پاسیو شخصی سرپوشیده که عکسش و گذاشتم  دارای پنکه سقفی و شوفاژ و کمد دیواری. که میشه هم به عنوان  اتاق خواب هو انباری استفاده کرد که ۲۰ متر است</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>۱۴۰۰</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
+          <t>۱۳۸۷</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>۲</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>۲۵۰</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+          <t>۱۴۰</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>طبقه۱ از ۵</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>آسانسور</t>
+        </is>
+      </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
@@ -1475,12 +1510,17 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>اجاره اداری و تجاری</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>صنعتی، کشاورزی و تجاری</t>
+          <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>09124354634</t>
         </is>
       </c>
     </row>
@@ -1490,32 +1530,35 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>۷۵ متر ۲ خواب</t>
+          <t>آپارتمان۱۰۰ متری پردیس فاز ۸</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>۲,۲۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۲۳۰,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: ۷۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>مسعودیه</t>
+          <t>حکیمیه</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/۷۵-متر-۲-خواب_آپارتمان_تهران_مسعودیه_دیوار/gY9uXtxG</t>
+          <t>https://divar.ir/v/آپارتمان۱۰۰-متری-پردیس-فاز-۸_آپارتمان_تهران_حکیمیه_دیوار/gY9GpZ2A</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>پارکینگ  جدا محاسبه میشود</t>
+          <t>آپارتمان اجاره پردیس فاز ۸
+تمام واحدها سکونت دارند
+دسترسی نزدیک به فروشگاه و مجتمع تجاری</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>۱۴۰۰</t>
+          <t>۱۳۹۹</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1525,10 +1568,14 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>۷۵</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
+          <t>۱۰۰</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>طبقه۴ از ۴</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -1544,29 +1591,26 @@
           <t>آسانسور</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۲۹٬۳۳۳٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>قیمت کل۲٬۲۰۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>09392584450</t>
         </is>
       </c>
     </row>
@@ -1576,53 +1620,67 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>آپارتمان کلید نخورده ۱۲۰ متری</t>
+          <t>آپارتمان اداری، مناسب داروخانه، ۵۹ متر، آزادی</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>۳,۶۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>توافقی</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>نو</t>
+          <t>آذربایجان</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-کلید-نخورده-۱۲۰-متری_آپارتمان_تهران_خانی-آباد-نو_دیوار/gY9unN4q</t>
+          <t>https://divar.ir/v/آپارتمان-اداری-مناسب-داروخانه-۵۹-متر-آزادی_دفتر-کار-اتاق-اداری-و-مطب_تهران_آذربایجان_دیوار/gY0y4JkB</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>سلام.اپارتمان نوساز و کلید نخورده..کابینت ممبران درجه یک با گاز رومیزی و شیر آلات و......پکیج....نقاشی شده ....فول امکانت....دو واحدی بدون دیوار مشترک.....سالن و اتاق خواب  و آشپزخانه همه پرده خور و روشن و .....فیلم واحد موجوده ...</t>
+          <t>✅ نقشه شده 3D مناسب داروخانه، آماده اجرا
+✅ روبروی بیمارستان شهریار
+✅ ۶ پزشک فعال نزدیک (متخصص اطفال، جراح و متخصص زنان، جراح و متخصص کلیه و مجاری ادراری، عمومی)
+✅ ۵۶ متر سند اداری
+✅ محل مناسب برای نصب تابلو
+✅ نبش کوچه ایستگاه بی آر تی
+✅ بسیار پر رفت و آمد
+✅ روبروی وزارت کار و امور اجتماعی
+✅ روبروی اداره تامین اجتماعی
+✅ ۶ متر انباری مجزا
+✅ دارای ۳ کولر اسپیلت
+✅ درب ضد سرقت
+✅ آیفون تصویری
+✅ کف سنگ
+✅ آسانسور فعال</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>۱۴۰۰</t>
+          <t>۱۳۹۱</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>۱۲۰</t>
+          <t>۵۹</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>انباری ندارد</t>
+          <t>انباری</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>پارکینگ</t>
+          <t>پارکینگ ندارد</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1630,14 +1688,10 @@
           <t>آسانسور</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۳۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
-          <t>قیمت کل۳٬۶۰۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کلتوافقی</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1647,12 +1701,17 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>فروش اداری و تجاری</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>دفتر کار، اتاق اداری و مطب</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>09359250619</t>
         </is>
       </c>
     </row>
@@ -1662,28 +1721,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>آپارتمان ۶۵متر  دو خوابه</t>
+          <t>اپارتمان 58مترتکواحدی فول ط1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ودیعه: ۳۰۰,۰۰۰,۰۰۰ تومان
-اجاره ماهیانه: ۳,۰۰۰,۰۰۰ تومان</t>
+          <t>۲,۰۵۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>الملک</t>
+          <t>پرستار</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۶۵متر-دو-خوابه_آپارتمان_تهران_خواجه-نظام-الملک_دیوار/gYzSyhcL</t>
+          <t>https://divar.ir/v/اپارتمان-58مترتکواحدی-فول-ط1_آپارتمان_تهران_پرستار_دیوار/gY9G5Wds</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>آپارتمان ۶۵متر  دوخوابه نبش ۴راه نورگیر عالی موقعیت اداری مسکونی مناسب دفتر کار خانواده و آرایشگاه .  انباری دارد حیاط پشت ساختمان برای نگهداری موتور مناسب است</t>
+          <t>پرستار سماواتیان58متر تکواحدی طبقه اول، فول، 20متر پارکینگ، 5متر انباری، بالکن، ایفون، تصویری،تخلیه،</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1693,19 +1751,15 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>۶۵</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>طبقه۳ از ۳</t>
-        </is>
-      </c>
+          <t>۵۸</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -1713,7 +1767,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>پارکینگ ندارد</t>
+          <t>پارکینگ</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1721,21 +1775,34 @@
           <t>آسانسور ندارد</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۳۵٬۳۴۴٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>قیمت کل۲٬۰۵۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>09125353128</t>
         </is>
       </c>
     </row>
@@ -1745,35 +1812,37 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>آپارتمان ۶۳ متری  مهندس معروف سازنده بنام منطقه</t>
+          <t>آپارتمان با پارکینگ و انباری تک واحدی تخلیه</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>۱,۱۷۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۳۱۵,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: مجانی</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>دولتخواه</t>
+          <t>تسلیحات</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۶۳-متری-مهندس-معروف-سازنده-بنام-منطقه_آپارتمان_تهران_دولتخواه_دیوار/gY8aVVzc</t>
+          <t>https://divar.ir/v/آپارتمان-با-پارکینگ-و-انباری-تک-واحدی-تخلیه_آپارتمان_تهران_تسلیحات_دیوار/gYh65pK-</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>کل ساختمان ۸ واحد ساختمان در بهترین لوکیشن اسماعیل آباد قرار دارد داخل کوچه نیست نبش کوچه روبروی پارک موقعیت عالی مترو دو دقیقه بی آر تی ۲ دقیقه فاصله دارد ساختمان دونبش می باشد فروش به دلیل خرید واحد بزرگتر سندآزاد
-ادرس اسماعیل إباد خ حیدری نبش اسکندری
-رهن ٢٢٠ملیون
-وام٤٨٠ملیون</t>
+          <t>آپارتمان،۳۸ متر،تک واحدی،با پارکینگ و انباری،اسپلیت،پکیج،گاز رومیزی،تخت تاشو،کمددیواری،
+سرویس حمام و دستشویی جدا،دستشویی فرنگی
+برای هماهنگی با شماره زیر تماس بگیرید
+09220590163
+،باتشکر</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>۱۳۹۲</t>
+          <t>۱۳۹۵</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1783,10 +1852,14 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>۶۳</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr"/>
+          <t>۳۸</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>طبقه۴ از ۴</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -1799,32 +1872,29 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۱۸٬۵۷۱٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>قیمت کل۱٬۱۷۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>09220590163</t>
         </is>
       </c>
     </row>
@@ -1834,100 +1904,64 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>آپارتمان ۷۰ متری خوش نقش دوخوبه</t>
+          <t>اجاره سوییت مبله ، آپارتمان ، منزل ، خانه مبله</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>۱,۴۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>اجاره روزانه: ۴۵۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>مسعودیه</t>
+          <t>جیحون</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۷۰-متری-خوش-نقش-دوخوبه_آپارتمان_تهران_مسعودیه_دیوار/gY9y3k3J</t>
+          <t>https://divar.ir/v/اجاره-سوییت-مبله-آپارتمان-منزل-خانه-مبله_آپارتمان-و-سوئیت_تهران_جیحون_دیوار/gYkIXp36</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>**فروشنده ۱۰۰ در صد **
-#خیابان رحیمی پلاک ۳۹ طبقه۳ سندی با انباری #
-٪اپارتمان ۷۰ متر ۲ خواب بدون یک سانت پرتی٪
-*قیمت یک میلیاردو چهارصدمیلیون تومان*
-#ساختمان ۸واحدهرطبقه ۲واحدی می باشدنما سنگ#
-*کابینت ام دی اف /کفپوش سرامیک/دارای بالکن وکمد دیواری*
-توجه ۳۰۰ میلیون رهن
-   ۴۸۰       میلیون وام
-۶۸۰    میلیون نقدی
-واحد مذکور نزدیک نزدیک خیابان ابومسلم خراسانی 
-* ایستگاه مترو   ۱۰۰ متری
-** آژانس توریستی محمود   ۱۵۰ متری
-***  ایستگاه اتوبوس    ۱۰۰ متری
-#  تربار   ۱۰۰  متری
-##  درمانگاه شبانه روزی    ۱۵۰ متری
-###  مدرسه    ۱۰۰ متری
-می باشد.
-شماره تماس:۰۹۱۹۱۱۲۴۸۴۴</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>۱۳۹۸</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>۲</t>
-        </is>
-      </c>
+          <t>//بیانه نمیخوام چون کلاه بردار نیستم.//
+فول امکانات زندگی
+خارج از طرح ترافیک
+در محله ای کاملا امن و آرام
+هفتگی ، ماهانه</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>۷۰</t>
+          <t>۴۰</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>پارکینگ ندارد</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>آسانسور ندارد</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۲۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>قیمت کل۱٬۴۰۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره کوتاه مدت</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>آپارتمان و سوئیت</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>09362651760</t>
         </is>
       </c>
     </row>
@@ -1937,42 +1971,52 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>اجاره آپارتمان مبله ۳خواب میرداماد شیک بی واسطه</t>
+          <t>اجاره انبار کانتینری ۱۳ متری مسقف در شرق تهران</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>اجاره روزانه: ۱,۵۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: توافقی
+اجاره ماهیانه: توافقی</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>میرداماد</t>
+          <t>حکیمیه</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اجاره-آپارتمان-مبله-۳خواب-میرداماد-شیک-بی-واسطه_آپارتمان-و-سوئیت_تهران_میرداماد_دیوار/QYHy6IYa</t>
+          <t>https://divar.ir/v/اجاره-انبار-کانتینری-۱۳-متری-مسقف-در-شرق-تهران_صنعتی-کشاورزی-و-تجاری_تهران_حکیمیه_دیوار/gYLEJdYb</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>اجاره آپارتمان مبله ۱۲۵ متری دو خواب میرداماد 
-نزدیک شریعتی 
-با تمام امکانات رفاهی 
-آسانسور  و پارکینگ 
-دسترسی آسان به مراکز خرید و درمانی
-دسترسی آسان به مترو شریعتی
-دارای سرایدار مقیم 
-رزرو ساعت ۱۱ الی ۱بامداد
-مهندس نظامدوست</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+          <t>اجاره انبار مسقف داخل سالن و سوله سرپوشیده در شرق تهران محدوده تهرانپارس، حکیمیه،سرخه حصار، افسریه و مسعودیه و خاوران
+انبارهای کانتینری داخل سوله مسقف بهترین و مقرون به صرفه ترین گزینه برای نگهداری موقت و طولانی مدت کالا ، جهیزیه و لوازم منزل و اثاثیه می باشد.
+ این انبارها در برابر گرمای تابستان و سرمای زمستان و اثرات آفتاب و برف و باران و گرد و خاک و طوفان مصون بوده ودارای محافظت دو چندان می باشد
+اجاره انبارهای کوچک مخصوص نگهداری اسباب و اثاثیه و کالای تجاری در کانتینرهای داخل سوله، با قیمت مقرون به صرفه در محدوده شرق تهران
+دارای انبارهای اختصاصی 20 فوت ( با ظرفیت یک خاور اتوبار و باربری) : فضای اجاره شده کاملا در اختیار مستاجر است و قفل شخصی خود را بر آن زده و کلید را با خود میبرد.
+انبار با سایز بزرگتر نیز جهت اجاره موجود میباشد
+انبار دارای حراست،واحد انتظامات، نگهبانان 24 ساعته و دوربین مداربسته دید در شب و برجکهای نگهبانی در امن ترین انبار محدوده جنوب شرق می باشد.
+دارای مجوز اتحادیه و انبار دارای بیمه آتش سوزی
+تلفن انبار : ۷۷۳۰۴۸۲۲
+۰۹۱۲۳۰۸۰۰۴۰</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>۱۴۰۰</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>۱۲۵</t>
+          <t>۱۳</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1988,12 +2032,17 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>اجاره کوتاه مدت</t>
+          <t>اجاره اداری و تجاری</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>آپارتمان و سوئیت</t>
+          <t>صنعتی، کشاورزی و تجاری</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>09123080040</t>
         </is>
       </c>
     </row>
@@ -2003,55 +2052,49 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>فروش آپارتمان منطقه 22 شهرک شهید خرازی</t>
+          <t>۶۳متر یکخواب بلوار ۱۳۱</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>۳,۴۱۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۲,۲۴۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>آزاد</t>
+          <t>شرقی</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/فروش-آپارتمان-منطقه-22-شهرک-شهید-خرازی_آپارتمان_تهران_سرو-آزاد_دیوار/gY9ynqnl</t>
+          <t>https://divar.ir/v/۶۳متر-یکخواب-بلوار-۱۳۱_آپارتمان_تهران_تهرانپارس-شرقی_دیوار/gY4ugrkf</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>سلام
-فروش آپارتمان با نازلترین قیمت شهر تهران
-اما بهترین منطقه آب و هوایی تهران
-شمال غربی ترین نقطه شهر
-دسترسی به شاهراه های شهر .اتوبان شهید همت و حکیم
-دسترسی به مترو
-در جوار ایرانمال بیمارستان تریتا شهر بازی در حال احداث هزار و یک شهر
-فقط فقط با شماره 9032989920 تماس بگیرید
-نهصد و سه دویست و نود و هشت نود و نه بیست
-برج های زیبا
-طبقه نهم شمال شرقی آفتابگیر
-تحویل موقت شده
-در صورت خرید کلید تحویل می گردد و در تعاونی بعد از  وکالت محضری به نام خریدار ثبت خواهد شد
-سند 6 دانگ به نام خریدار در آینده ای نزدیک</t>
+          <t>۶۳ متر  یک خواب 
+بلوار  ۱۳۱ خیابان شهابی 
+۲ طرف  نور 
+با  انباری  اسانسور 
+خوش  نقشه 
+حدود  ۱۶  ساله تمیز 
+تخلیه 
+۱۰متر  حیاط خلوت قابل مسقف کردن و استفاده شخصی  این واحد</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>۱۴۰۰</t>
+          <t>۱۳۸۴</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>۱۱۰</t>
+          <t>۶۳</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -2062,7 +2105,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>پارکینگ</t>
+          <t>پارکینگ ندارد</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -2072,12 +2115,12 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>قیمت هر متر۳۱٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت هر متر۳۵٬۵۵۵٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>قیمت کل۳٬۴۱۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کل۲٬۲۴۰٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2093,6 +2136,11 @@
       <c r="R20" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>09014254864</t>
         </is>
       </c>
     </row>
@@ -2102,48 +2150,48 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>اپارتمان دوخوابه دروس</t>
+          <t>آپارتمان ۶۱متری خوش نقشه تخلیه</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ودیعه: ۵۰۰,۰۰۰,۰۰۰ تومان
-اجاره ماهیانه: ۱۸,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۱۶۰,۰۰۰,۰۰۰ تومان
+اجاره ماهیانه: ۲,۵۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>دروس</t>
+          <t>مسعودیه</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اپارتمان-دوخوابه-دروس_آپارتمان_تهران_دروس_دیوار/gY9u3PAQ</t>
+          <t>https://divar.ir/v/آپارتمان-۶۱متری-خوش-نقشه-تخلیه_آپارتمان_تهران_مسعودیه_دیوار/gY9GpEzu</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>دروس یارمحمدی اپارتمان دوخوابه با اسانسور انباری پارکینگ استخر سونا جکوزی</t>
+          <t>باسلام واحد فوق درکوچه رحیمی ساختمان عالی باهمسایگان بسیارخوب کف سرامیک کمددیواری بزرگ اتاق خواب بزرگ پذیرایی بزرگ چیدمان عالی نور عالی بالکن داردانباری بزرگ جای پارک موتور دارد ماشین جلوی درب جای پارک دارد درکل ساختمان ساکت آرامی هستش تخلیه فوری بازدید ساعت ۱۱ الی ۱۳ و۱۶الی ۲۰</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>۱۳۸۵</t>
+          <t>۱۳۸۷</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>۱۱۲</t>
+          <t>۶۱</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>طبقه۵ از ۵</t>
+          <t>طبقه۳</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2153,12 +2201,12 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>پارکینگ</t>
+          <t>پارکینگ ندارد</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>آسانسور</t>
+          <t>آسانسور ندارد</t>
         </is>
       </c>
       <c r="N21" t="inlineStr"/>
@@ -2176,6 +2224,11 @@
       <c r="R21" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>09190137507</t>
         </is>
       </c>
     </row>
@@ -2185,42 +2238,42 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>آپارتمان ۵۹ متر ۱ خواب  مناسب مطب و دفتر کار</t>
+          <t>آپارتمان ۷۰متر ۲ خواب</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>توافقی</t>
+          <t>۲۳۸,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>لومومبا</t>
+          <t>منیریه</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۵۹-متر-۱-خواب-مناسب-مطب-و-دفتر-کار_آپارتمان_تهران_پاتریس-لومومبا_دیوار/gY9uHIMp</t>
+          <t>https://divar.ir/v/آپارتمان-۷۰متر-۲-خواب_آپارتمان_تهران_منیریه_دیوار/gY9G5BZ0</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>واحد کامل بازسازی شده مناسب دفتر کار قابل تبدیل به ۲ خواب ساختمان کامل امن دارای نگهبانی ۲۴ ساعته و.....</t>
+          <t>نزدیک به مترو و بی ارتی خیابان اصلی و مرکز خرید</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>۱۳۹۱</t>
+          <t>۱۳۹۰</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>۱</t>
+          <t>۲</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>۵۹</t>
+          <t>۷۰</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -2231,18 +2284,22 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>پارکینگ</t>
+          <t>پارکینگ ندارد</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr"/>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۳٬۴۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>قیمت کلتوافقی</t>
+          <t>قیمت کل۲۳۸٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2258,6 +2315,11 @@
       <c r="R22" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>09120919223</t>
         </is>
       </c>
     </row>
@@ -2267,72 +2329,84 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>دربست حیاط دار</t>
+          <t>آپارتمان ۱۲۲متری دو واحدی</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ودیعه: ۱۳۰,۰۰۰,۰۰۰ تومان
-اجاره ماهیانه: ۳,۵۰۰,۰۰۰ تومان</t>
+          <t>توافقی</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>استخر</t>
+          <t>شریعتی</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/دربست-حیاط-دار_خانه-و-ویلا_تهران_استخر_دیوار/gY9yHPBY</t>
+          <t>https://divar.ir/v/آپارتمان-۱۲۲متری-دو-واحدی_آپارتمان_تهران_شهرک-شریعتی_دیوار/gYhqaQ3H</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>فقط تماس بگیرین تا 10 شب</t>
+          <t>آپارتمان طبقه ۶ است.مشرف نداره ساختمانهای اطراف ۴ طبقه اس.تراس بزرگ داره.رنگ شده.پکیج و رادیاتور نصب شده.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>۱۳۹۰</t>
+          <t>۱۴۰۰</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>۱</t>
+          <t>۲</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>۷۰</t>
+          <t>۱۲۲</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>انباری</t>
+          <t>انباری ندارد</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>پارکینگ ندارد</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
+          <t>پارکینگ</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>آسانسور</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>قیمت کلتوافقی</t>
+        </is>
+      </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>خانه و ویلا</t>
+          <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>09125886567</t>
         </is>
       </c>
     </row>
@@ -2342,52 +2416,69 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>سه دانگ حجره در فاز یک</t>
+          <t>63متر</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>۳۰,۰۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۲,۲۵۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>شریعتی</t>
+          <t>کرمان</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/سه-دانگ-حجره-در-فاز-یک_مغازه-و-غرفه_تهران_شهرک-شریعتی_دیوار/gY9ynIEg</t>
+          <t>https://divar.ir/v/63متر_آپارتمان_تهران_کرمان_دیوار/gY9CJzgq</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>سه دانگ حجره در فاز یک سالن ۱۱ روبه ۱۲ حجره ۸ به فروش میرسد قیمت یک کلام ۳۰تومن</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>لطفا جهت بازدید با شماره
+09900031975تماس بگیرید</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>۱۳۸۵</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>۳۰۰</t>
+          <t>۶۳</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>انباری</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>قیمت هر متر۱۰۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت هر متر۳۵٬۷۱۴٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>قیمت کل۳۰٬۰۰۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کل۲٬۲۵۰٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2397,12 +2488,17 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>فروش اداری و تجاری</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>مغازه و غرفه</t>
+          <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>09354265967</t>
         </is>
       </c>
     </row>
@@ -2412,61 +2508,53 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>آپارتمان ۷۷ متری میدان کمال الملک تهرانسر</t>
+          <t>50 متری پارکینگ اسانسور</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>۳,۰۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۱,۱۲۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>تهران‌سر</t>
+          <t>فلاح</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۷۷-متری-میدان-کمال-الملک-تهرانسر_آپارتمان_تهران_تهران-سر_دیوار/gYxGdkNJ</t>
+          <t>https://divar.ir/v/50-متری-پارکینگ-اسانسور_آپارتمان_تهران_فلاح_دیوار/gY9-YmMf</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>بهترین نقطه تهرانسر
-غرق نور 
-خوش نقشه
-دولاین آسانسور
-بازسازی شده
-چشم انداز عالی 
-دارای ۳ اسپیلت مجزای سرد و گرم
-بالکن از دو طرف
-از دو طرف نورگیر
-سالن پرده خور
-کاغذ دیواری
-اجاق رومیزی
-کمد دیواری
-سند آزاد آماده محضر</t>
+          <t>فول
+اسانسور
+پارکینگ
+پارکینگ جداگانه 100 ت 
+فایل شخصی
+املاک به هیچ عنوان تماس نگیرد</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>۱۳۸۳</t>
+          <t>۱۳۹۳</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>۷۷</t>
+          <t>۴۸</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>انباری</t>
+          <t>انباری ندارد</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2481,12 +2569,12 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>قیمت هر متر۳۸٬۹۶۱٬۰۰۰ تومان</t>
+          <t>قیمت هر متر۲۳٬۳۳۳٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>قیمت کل۳٬۰۰۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کل۱٬۱۲۰٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2502,6 +2590,11 @@
       <c r="R25" t="inlineStr">
         <is>
           <t>آپارتمان</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>09028873711</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
scraper and site are working gine
</commit_message>
<xml_diff>
--- a/divar.xlsx
+++ b/divar.xlsx
@@ -531,96 +531,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>اپارتمان(فول امکانات)</t>
+          <t>پیش فروش برج وزرا / مروارید شهر</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>توافقی</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ر   ن ی ا و ر ا ن</t>
+          <t>چیتگر</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اپارتمان-فول-امکانات-_آپارتمان_تهران_نیاوران_دیوار/gYBb5qLi</t>
+          <t>https://divar.ir/v/پیش-فروش-برج-وزرا-مروارید-شهر_پیش-فروش_تهران_چیتگر_دیوار/gYB7HCqM</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>✖عجله کن تا از دستش ندادی✖
-⭐میخای سرمایه گذاری کنی؟
-⭐میخای سکونت کنی؟
-❎یک مورد عالی برات دارم
-⭐یک انتخاب درست زندگیتو متحول میکنه
-❎فروش کامل❎️
-⭐برج مسکونی سوپر لاکچری کلید نخورده
-✔٢٥٠٠ متر زمین
-✔️١٩٠٠٠ متر بنای کل
-✔️١٣٠٠٠ متر بنای مفید
-✔پنت هاوس ١٠٠٠ متری
-⭐4خواب مستر + سوئیت مجزا
-⭐دارای ٩٥ پارکینگ سندی
-✔دارای ٢٠ انباری به متراژ 20متر
-⭐دارای ژنراتور ٤٥٠ کیلوواتی
-❎مشاعات؛
-✖استخر ، سونای خشک و بخار
-✖آرایشگاه مردانه و زنانه 
-✖اتاق اپیلاسیون 
-✖سالن ورزشی 
-⭐سالن اجتماعات به مساحت ٤٠٠ متر دارای ٢ ورودی مجزا و سرویس بهداشتی و رختکن
-✔لابی به مساحت ٦٠٠ متر
-⭐دارای کانتر لابی من
-✔کافی شاپ مبله با مبلمان و لوستر ورساچه
-✔واحد پنت هاوس دارای استخر و سونا و جکوزی اختصاصی
-⭐دارای ٣ درب ورودی با چوب افریقایی به ارتفاع ٩ متر
-⭐٣ لاین آسانسور 
-دو لاین ١٢نفره و 
-یک لاین ١٨ نفره
-✔سند شش دانگ بدون ریشه و مشکل
-⭐برگه عدم خلاف و پایان کار
-✔بعد از عقد قرارداد آماده تحویل می باشد
-❎قیمت امضا 2350 میلیارد
-متری 190میلیون
-تخفیف عالی برای مشتری واقعی</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>۱۳۹۸</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>+۴</t>
-        </is>
-      </c>
+          <t>پیش فروش تعداد محدودی از واحدهای برج وزرا
+مناسب جهت سرمایه گذاری و سکونت
+پروژه دارای سند تک برگ و جواز ساخت
+هدف ما تحقق رویای شماست
+متراژ واحدها
+110 متر دو خواب
+125 متر سه خواب
+150 متر سه خواب
+اختصاری از امکانات برج
+استخر سونا جکوزی روف گاردن کتابخانه سالن اجتماعات سالن کودک سیستم هوشمند BMS اتاق نمک و .....
+پیش پرداخت فقط 340 م تومان
+تحویل 36 ماهه 
+دارای نمونه ساخت در منطقه جهت بازدید
+با قید تعهد ضرر و زیان در صورت تاخیر در تحویل پروژه
+تراکم متری 9.100
+به صورت مستقیم از تعاونی خرید کنید
+کارگزار رسمی تعاونی</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>قیمت کلتوافقی</t>
-        </is>
-      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
           <t>sell</t>
@@ -628,12 +586,12 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>پرو‌ژه‌های ساخت و ساز</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>پیش‌فروش</t>
         </is>
       </c>
       <c r="S2" t="inlineStr"/>
@@ -644,59 +602,81 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>خانه کلنگی ۶۹ متری</t>
+          <t>آپارتمان ۴۶ متری ‌بهر خیابان اصلی</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>۲,۵۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۲۶۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ر   و ح ی د ی ه</t>
+          <t>مقدم</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/خانه-کلنگی-۶۹-متری_زمین-و-کلنگی_تهران_وحیدیه_دیوار/gYBXJ8zP</t>
+          <t>https://divar.ir/v/آپارتمان-۴۶-متری-بهر-خیابان-اصلی_دفتر-کار-اتاق-اداری-و-مطب_تهران_مقدم_دیوار/gYBjKPSf</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>فقط برای فروش در خدمتم.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+          <t>رهن کامل ۲۶۰ 
+کف سرامیک 
+تازه بازسازی شد
+نزدیک ایستگاه اتوبوس و مترو 
+بهر خیابان اصلی ابوذر 
+باتمام امکانات آب برق گاز تلفن 
+طبقه همکف</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>۱۳۷۵</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>۴۶</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۳۴٬۷۸۲٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>قیمت کل۲٬۴۰۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره اداری و تجاری</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>زمین و کلنگی</t>
+          <t>دفتر کار، اتاق اداری و مطب</t>
         </is>
       </c>
       <c r="S3" t="inlineStr"/>
@@ -707,47 +687,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>آپارتمان 60 متری فول موقعیت اداری واقع در 196</t>
+          <t>آپارتمان دو خوابه</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ودیعه: ۳۹۵,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۵۲۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ر   ت ه ر ا ن پ ا ر س   ش ر ق ی</t>
+          <t>باغ فیض</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-60-متری-فول-موقعیت-اداری-واقع-در-196_آپارتمان_تهران_تهرانپارس-شرقی_دیوار/gYAfzk6r</t>
+          <t>https://divar.ir/v/آپارتمان-دو-خوابه_آپارتمان_تهران_باغ-فیض_دیوار/gYBjalO5</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>موقعیت اداری 
-فول امکانات 
-قابل تبدیل تا 300 م 
-محیط مناسب برای کار 
-وکالت 
-پزشکی
-دندانپزشکی 
-مدیریت بسیار قوی
-سالن فلات با قابلیت پارتیشن بندی
-لوکیشن عالی در خیابان اصلی
-  املاکی محترم تماس نگیرید</t>
+          <t>از سه طرف نورگیر</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>۱۳۸۷</t>
+          <t>۱۳۸۵</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>۱</t>
+          <t>۲</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -757,7 +727,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>طبقه۴ از ۵</t>
+          <t>طبقه۱</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -772,7 +742,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>آسانسور</t>
+          <t>آسانسور ندارد</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
@@ -800,49 +770,78 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>زمین برای مشارکت</t>
+          <t>55متر پاسدارگمنام قیام جنوبی</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>۱,۸۳۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ر   س ع ا د ت ‌ آ ب ا د</t>
+          <t>پیروزی</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/زمین-برای-مشارکت_مشارکت-در-ساخت_تهران_سعادت-آباد_دیوار/gYBbZkKL</t>
+          <t>https://divar.ir/v/55متر-پاسدارگمنام-قیام-جنوبی_آپارتمان_تهران_پیروزی_دیوار/gYBj6cf8</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>زمین جنگلی جهت مشارکت در ساخت 
-حیاط اطراف زمین کاملا جنگل 
-نیم ساعت فاصله تا دریا 
-کمتر از ١٠ دقیقه تا مرکز شهر 
-۵ دقیقه فاصله تا مراکز خرید جدید و مدرن 
-آب چشمه 
-ویو ابدی شهر و جنگل 
-لوکیشن تاپ و بی نظیر 
-بدون مشابه 
-مدارک کامل 
-سند در حال صدور 
-منطقه بسیار زیبا و آرامش محض</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+          <t>55متر فول باز سازی
+تک واحدی. کف پارکت لمینت برند هاوس بادن متری 470زدم با5سال گارانتی
+کابینت ها پله ای و مدرن که این نوع کابینت گرون ترین نوع کابینت هست ورق ها و لولا ها 10سال گارانتی شرکتی داره زیر سینکpvcهست
+یک نمای پارتیشنی بسیار شیک کار شده
+کاشی سرویس ها همگی البرز هست و عالی و مدرن کار شده همراه با روشویی سنگی. درب های اتاق خواب و ورودی و سرویس از جنس چو ب گردو. کاغذ دیواری خارجی رولی 600هزینه کردم
+شیرآلات کامل تعویض شده. واحد کاملا شیک و اسپرت سبک روستیک کار شده
+بهترین کوچه قیام. شاهد 12.دسترسی به متروپیاده 5مین. دسترسی به امام علی و محلاتی
+لوکیشن واحد فوقالعادس. نور گیر هم از پذیرایی هم از اتاق خواب هم از آشپزخونه
+اطلاعات بیشتر فقط تماس. با تشکر</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>۱۳۷۹</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>۵۵</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>انباری</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۳۳٬۲۷۲٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>قیمت کل۱٬۸۳۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr">
         <is>
           <t>sell</t>
@@ -850,12 +849,12 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>پرو‌ژه‌های ساخت و ساز</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>مشارکت در ساخت</t>
+          <t>آپارتمان</t>
         </is>
       </c>
       <c r="S5" t="inlineStr"/>
@@ -866,49 +865,47 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>آپارتمان ۶۴ متری ۲ خواب شهرک مریم</t>
+          <t>پارگینگ اجاره ای</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>۱,۳۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۵۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ر   ا ن د ی ش ه</t>
+          <t>امیریه</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۶۴-متری-۲-خواب-شهرک-مریم_آپارتمان_تهران_اندیشه_دیوار/gYBbZPHs</t>
+          <t>https://divar.ir/v/پارگینگ-اجاره-ای_آپارتمان_تهران_امیریه_دیوار/gYBjqjoK</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>بهترین موقعیت شهرک 
-بسیار خوش نقشه و شیک
-سازنده بنام شهرک
-پارکینگ اختصاصی
-دسترسی به طالقانی و شهرک</t>
+          <t>40مترپارکینگ  
+دارای سرویس بهداشتی
+جهت انباری</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>۱۳۹۲</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>۲</t>
-        </is>
-      </c>
+          <t>۱۳۸۵</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>۶۴</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
+          <t>۴۰</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>طبقهزیرهمکف</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -924,24 +921,16 @@
           <t>آسانسور ندارد</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۲۰٬۳۱۲٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>قیمت کل۱٬۳۰۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -957,32 +946,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>دفتر کار نقلی آدرس و موقعیت</t>
+          <t>آپارتمان 60 متری یک خوابه</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>توافقی</t>
+          <t>۲۸۵,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ر   د ر د ش ت</t>
+          <t>سرآسیاب دولاب</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/دفتر-کار-نقلی-آدرس-و-موقعیت_دفتر-کار-اتاق-اداری-و-مطب_تهران_دردشت_دیوار/gYBb5RXq</t>
+          <t>https://divar.ir/v/آپارتمان-60-متری-یک-خوابه_آپارتمان_تهران_سرآسیاب-دولاب_دیوار/gYBjahBm</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>سلام دوستان تو منطقه نوساز اداری ۶۵ تا ۷۰ خرید و فروش میشه من با خریدار واقعی تخفبف خوب میدم ملک نقلی و به قیمت برای دفتر کار عالیه ساختمان خلوت و همسایه های محترم و مدیریت قوی در خدمت دوستان هستم</t>
+          <t>دسترسی سریع به مترو پیروزی نزدیک میدان تره بار ساختمان خلوت تک واحدی نورگیر عالی روشن و تمیز رنگ تازه شده</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>۱۳۸۰</t>
+          <t>۱۳۹۱</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -992,13 +981,13 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>۳۶</t>
+          <t>۶۰</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>انباری ندارد</t>
+          <t>انباری</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1008,13 +997,17 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr"/>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۴٬۷۵۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>قیمت کلتوافقی</t>
+          <t>قیمت کل۲۸۵٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,12 +1017,12 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>فروش اداری و تجاری</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>دفتر کار، اتاق اداری و مطب</t>
+          <t>آپارتمان</t>
         </is>
       </c>
       <c r="S7" t="inlineStr"/>
@@ -1040,27 +1033,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>۱۲۰متری زیربنای خانه ۸۵متری 'وطبقه ونیم</t>
+          <t>۱۰۰ متر دفتر کار یا کارگاه ب مشاغل بی سروصدا .</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>توافقی</t>
+          <t>ودیعه: ۴۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ر   ف ی ر و ز آ ب ا د ی</t>
+          <t>پیروزی</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/۱۲۰متری-زیربنای-خانه-۸۵متری-وطبقه-ونیم_خانه-و-ویلا_تهران_فیروزآبادی_دیوار/gYBbZKJf</t>
+          <t>https://divar.ir/v/۱۰۰-متر-دفتر-کار-یا-کارگاه-ب-مشاغل-بی-سروصدا-_دفتر-کار-اتاق-اداری-و-مطب_تهران_پیروزی_دیوار/gYBb6yRw</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ادرس شهرری:میدان عبدالعظیم خیابان قدمی کوچه زارع اردستانی کوچه مختارخان پلاک ۸۵طبقه دوم</t>
+          <t>۱۰۰ متر دفتر کار یا کارگاه .ب مشاغل بی صدا .درب مستقل .باسازی شده .بهترین مکان جهت دفتر کار یا کارگاه.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1070,12 +1063,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>۱</t>
+          <t>۲</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>۸۵</t>
+          <t>۱۰۰</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -1089,22 +1082,26 @@
           <t>پارکینگ ندارد</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره اداری و تجاری</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>خانه و ویلا</t>
+          <t>دفتر کار، اتاق اداری و مطب</t>
         </is>
       </c>
       <c r="S8" t="inlineStr"/>
@@ -1115,68 +1112,75 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>مغازه پر مشتری و</t>
+          <t>آپارتمان سند اداری - فلت</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>توافقی</t>
+          <t>ودیعه: ۱,۰۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ر   ت ه ر ا ن پ ا ر س   ش ر ق ی</t>
+          <t>نیلوفر</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/مغازه-پر-مشتری-و_مغازه-و-غرفه_تهران_تهرانپارس-شرقی_دیوار/gYo-Xz-r</t>
+          <t>https://divar.ir/v/آپارتمان-سند-اداری-فلت_دفتر-کار-اتاق-اداری-و-مطب_تهران_نیلوفر_دیوار/gYBbKYMC</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>با سلام مغازه فوق فوری به فروش میرسد 
-مغازه محدوده بسیار عالی در تهرانپارس شرقی است 
-حداقل ۵۰۰تا مشتری ثابت داره چون حدود ۱۵ساله سابقه کارداره دارای اب برق گاز و خط تلفن است
-ملکیت است بالای مغازه قابل ساخت هست 
-چال دارد،به دلیل خرید ملک میفروشم وگرنه پاخورش عالیه و این که مشتری خودشو داره مغازه الان دسته اجاره هستش که بهم درصد میده،شماام میتونید اجاره بدین که بهتون درصد بده چون مغازه مشتری ثابت داره
-فوری</t>
+          <t>طبقه 4 تک واحدی  - دو خواب نورگیری عالی - نبش قندی - دسترسی بسار خوب - بازسازی کامل</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>۱۳۸۵</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
+          <t>۱۳۸۸</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>۲</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>۱۳</t>
+          <t>۱۱۴</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>پارکینگ</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>آسانسور</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>قیمت کلتوافقی</t>
-        </is>
-      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>فروش اداری و تجاری</t>
+          <t>اجاره اداری و تجاری</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>مغازه و غرفه</t>
+          <t>دفتر کار، اتاق اداری و مطب</t>
         </is>
       </c>
       <c r="S9" t="inlineStr"/>
@@ -1187,51 +1191,77 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>اجاره سوییت و آپارتمان مبله</t>
+          <t>آپارتمان ۶۰ متری وصفنارد</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>۱,۲۱۸,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ر   ص ا د ق ی ه</t>
+          <t>وصفنارد</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اجاره-سوییت-و-آپارتمان-مبله_آپارتمان-و-سوئیت_تهران_صادقیه_دیوار/gYWGwswa</t>
+          <t>https://divar.ir/v/آپارتمان-۶۰-متری-وصفنارد_آپارتمان_تهران_وصفنارد_دیوار/gYBjKP-p</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>بدون نیاز به بیعانه
-فاصله تا مترو یک دقیقه
-مستقیم با مالک بی واسطه
-کاملا ضدعفونی شده و کاملا تمیز
-دسترسی آسان
-لوکس و شیک
-پارکینگ و اسانسور
-نگهبانی 
-کوچه اختصاصی
-برای رزرو تماس بگیرید</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+          <t>آپارتمان ۶۰ متری تمیز 
+مشاعات سنگ و تمیز 
+چهار طبقه تک واحدی شخصی ساز 
+بهترین متریال 
+نور عالی 
+توالت ایرانی و فرنگی 
+کابینت ام دی اف 
+کف سرامیک</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>۱۳۹۵</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>۹۰</t>
+          <t>۵۸</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>آسانسور</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۲۱٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>قیمت کل۱٬۲۱۸٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr">
         <is>
           <t>sell</t>
@@ -1239,12 +1269,12 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>اجاره کوتاه مدت</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>آپارتمان و سوئیت</t>
+          <t>آپارتمان</t>
         </is>
       </c>
       <c r="S10" t="inlineStr"/>
@@ -1255,49 +1285,64 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>باغ لواسان بزرگ</t>
+          <t>آپارتمان ۶۰متری تک خواب</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>۷,۰۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>توافقی</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ر   پ ی ر و ز ی</t>
+          <t>بهمن یار</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/باغ-لواسان-بزرگ_زمین-و-کلنگی_تهران_پیروزی_دیوار/gYBbJXIW</t>
+          <t>https://divar.ir/v/آپارتمان-۶۰متری-تک-خواب_آپارتمان_تهران_بهمن-یار_دیوار/gYBjqZXQ</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>باغ لواسان بزرگ درخت آلبالو .گیلاس .گردو .آلوچه
-آب هوا خوب 
-سند پلاک ثبتی 
-1000متر متری 7میلیون
-در صورت معامله صحبت میکنیم 
-فقط پیام بدهید</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+          <t>آپارتمان تک خواب متراژ۲۴۰ متر</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>۱۳۷۵</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>۱</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>۶۰</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۷٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>انباری ندارد</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
-          <t>قیمت کل۷٬۰۰۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کلتوافقی</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1312,7 +1357,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>زمین و کلنگی</t>
+          <t>آپارتمان</t>
         </is>
       </c>
       <c r="S11" t="inlineStr"/>
@@ -1323,54 +1368,47 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>۷۵متر ۲خوابه فلکه اول ۱۳۸شرقی</t>
+          <t>ویلایی با موقعیت اداری</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ودیعه: ۲۵۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۱۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ر   ت ه ر ا ن پ ا ر س   غ ر ب ی</t>
+          <t>تهرانپارس غربی</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/۷۵متر-۲خوابه-فلکه-اول-۱۳۸شرقی_آپارتمان_تهران_تهرانپارس-غربی_دیوار/gYBbZUGw</t>
+          <t>https://divar.ir/v/ویلایی-با-موقعیت-اداری_دفتر-کار-اتاق-اداری-و-مطب_تهران_تهرانپارس-غربی_دیوار/gYBXK71a</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>سلام
-آپارتمان پنج طبقه دو واحدی 
-طبقه سوم فول امکانات 
-داخل واحد مدرن
-فلکه اول ۱۳۸شرقی 
-املاک</t>
+          <t>سالن زیبایی در بهترین لوکشین تهرانپارس 
+موقعیت اداری 
+با مشتری ثابت فقط با کلیه وسایل واگزار می شود .</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>۱۳۹۲</t>
+          <t>۱۳۷۲</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>۷۵</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>طبقه۳</t>
-        </is>
-      </c>
+          <t>۷۰</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -1383,7 +1421,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>آسانسور</t>
+          <t>آسانسور ندارد</t>
         </is>
       </c>
       <c r="N12" t="inlineStr"/>
@@ -1395,12 +1433,12 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>اجاره اداری و تجاری</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>دفتر کار، اتاق اداری و مطب</t>
         </is>
       </c>
       <c r="S12" t="inlineStr"/>
@@ -1411,83 +1449,68 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>آپارتمان 140 متر ویودار ازگل</t>
+          <t>اجاره سوپرمارکت با کلیه امکانات</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>۱۱,۲۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: توافقی</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ر   ا ز گ ل</t>
+          <t>بهاران</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-140-متر-ویودار-ازگل_آپارتمان_تهران_ازگل_دیوار/gYBbJEfe</t>
+          <t>https://divar.ir/v/اجاره-سوپرمارکت-با-کلیه-امکانات_مغازه-و-غرفه_تهران_بهاران_دیوار/gYBbqsPz</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>طبقه هشتم ویو وتور از جنوی و شمال با پارکینگ و اسانسور ودسترسی عالی به اتوبان ها و سند تک برگ</t>
+          <t>اجاره سوپرمارکت با امکانات کامل
+۵ عدد یخچال ایستاده 
+۲ عدد یخچال بستنی 
+دوربین 
+ترازو محک پالت 
+کالباس بر 
+ویترین 
+آب برق گاز تلفن سرویس بهداشتی 
+با دخل خوب ۲۰ سال سابقه سوپرمارکت 
+دونبش محلی با سوددهی عالی</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>۱۳۹۵</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>۳</t>
-        </is>
-      </c>
+          <t>۱۳۹۰</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>۱۴۰</t>
+          <t>۳۵</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۸۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>قیمت کل۱۱٬۲۰۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره اداری و تجاری</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>مغازه و غرفه</t>
         </is>
       </c>
       <c r="S13" t="inlineStr"/>
@@ -1498,89 +1521,67 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>آپارتمان ۷۷ متری پاسداران گلستان ۷ بازسازی شده</t>
+          <t>مغازه 10 متر اسلامشهر پاساژ</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ودیعه: ۱,۰۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۱,۲۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ر   پ ا س د ا ر ا ن</t>
+          <t>دولتخواه</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۷۷-متری-پاسداران-گلستان-۷-بازسازی-شده_آپارتمان_تهران_پاسداران_دیوار/gYBD5l4i</t>
+          <t>https://divar.ir/v/مغازه-10-متر-اسلامشهر-پاساژ_مغازه-و-غرفه_تهران_دولتخواه_دیوار/gYBjqTkD</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>فول امکانات
-۵ طبقه ۴ واحدی
-واحد طبقه اول
-تیکه اول پاسداران
-گلستان ۷ کوچه دنج و خلوت
-تخلیه
-تمیز - کاغذ دیواری و نقاشی شده
-دارای حیاط خلوت
-سالن و هردو اتاق خواب کولر گازی دارد
-واحد جنوبی ساختمان شمالی
-غیر قابل تبدیل</t>
+          <t>مغازه 10 متر اسلامشهر واوان پاساژ اکباتان 2 طبقه بالا راهرو پشت</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>۱۳۹۱</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>۲</t>
-        </is>
-      </c>
+          <t>۱۳۸۰</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>۷۷</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>طبقه۱</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+          <t>۱۰</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۱۲۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>قیمت کل۱٬۲۰۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>فروش اداری و تجاری</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>مغازه و غرفه</t>
         </is>
       </c>
       <c r="S14" t="inlineStr"/>
@@ -1591,52 +1592,56 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>اپارتمان۳۵متری نقلی خوش نقشه فتاحی</t>
+          <t>آپارتمان ۱۲۵ متری فول بازسازی شده</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ودیعه: ۲۵۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۴۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ر   س ب ل ا ن</t>
+          <t>شهرک فردوس</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اپارتمان۳۵متری-نقلی-خوش-نقشه-فتاحی_آپارتمان_تهران_سبلان_دیوار/gYBXJ9m9</t>
+          <t>https://divar.ir/v/آپارتمان-۱۲۵-متری-فول-بازسازی-شده_آپارتمان_تهران_شهرک-فردوس_دیوار/gYBjKOh1</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>واحد تمیز
-پذیرایی ۹متری
-سرویس جدا
-پله بزرگ
-سندی اول رویتی دوم
-بازدید ۶عصر ب بعد</t>
+          <t>مشاور املاک ارامش
+۱۲۵متر
+فول باز سازی شده مشابه نوساز
+جای دنج و ارام
+۲خوابه
+کابینت های کلاس
+شیر الات نو
+کف سرامیک
+ادرس املاک خیابان چهارده معصوم جنوبی پلاک ۳
+تلفن تماس:۰۹۱۲۷۹۹۷۸۸۵</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>۱۳۹۰</t>
+          <t>۱۳۷۱</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>۱</t>
+          <t>۲</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>۳۵</t>
+          <t>۱۲۵</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>طبقه۲ از ۴</t>
+          <t>طبقه۲ از ۳</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1646,7 +1651,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>پارکینگ ندارد</t>
+          <t>پارکینگ</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1679,47 +1684,50 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>250متر در سه طبقه بازسازی شده</t>
+          <t>آپارتمان مجیدیه فروش آپارتمان مجیدیه جنوبی حاجی پو</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ودیعه: ۹۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۱,۳۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ر   ا م ی ن   ح ض و ر</t>
+          <t>مجیدیه</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/250متر-در-سه-طبقه-بازسازی-شده_خانه-و-ویلا_تهران_امین-حضور_دیوار/gY-KJu-b</t>
+          <t>https://divar.ir/v/آپارتمان-مجیدیه-فروش-آپارتمان-مجیدیه-جنوبی-حاجی-پو_آپارتمان_تهران_مجیدیه_دیوار/gYL62DbS</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>بازسازی شده 
-کوچه ماشین رو خونه هم ماشین رو 
-مناسب برای سه خانواده 
-کابینت ممبران ،کولر گازی پکیج و رادیاتور
-هر طبقه 80متر 
-امکانات هر یک مجزا</t>
+          <t>داری یک اتاق ۹ متری و توافق شده ۶ متر نور گیر ساختمان را سقف زده و به واحد ملحق گردد. که در واقع واحد، ۲ خواب خواهد شد
+ کمد دیواری .شوفاژ . کابینت ام دی اف و گاز رومیزی، بالکن، سرویس و حمام جدا 
+ساختمان تمیز و بی سر وصدا و منظم 
+طبقه اول سندی و دوم رویتی 
+✔مجیدیه جنوبی بر کوچه صالحی  نزدیک خیابان حاجی پور 
+در صورت تمایل خریدار مالک رهن کامل به مبلغ ۱۸۰ میلیون خواهم کرد
+۲.۱۲ انباری سندی دارد و ۱.۳۰ بالکن 
+ که مجموع متراژ ۳۹ متر می باشد 
+#معاوضه با ملک موقعیت اداری $</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>۱۳۸۳</t>
+          <t>۱۳۸۲</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>+۴</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>۲۴۰</t>
+          <t>۳۹</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -1730,25 +1738,37 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+          <t>پارکینگ ندارد</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۳۳٬۳۳۳٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>قیمت کل۱٬۳۰۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>خانه و ویلا</t>
+          <t>آپارتمان</t>
         </is>
       </c>
       <c r="S16" t="inlineStr"/>
@@ -1759,83 +1779,57 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>آپارتمان ۹۰ متری در شکوفه</t>
+          <t>تک خواب باپارکینگ فول امکانات نمایشگاه</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>توافقی</t>
+          <t>اجاره روزانه: ۵۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ر   پ ی ر و ز ی</t>
+          <t>پاسداران</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۹۰-متری-در-شکوفه_آپارتمان_تهران_پیروزی_دیوار/gYBXp3RY</t>
+          <t>https://divar.ir/v/تک-خواب-باپارکینگ-فول-امکانات-نمایشگاه_آپارتمان-و-سوئیت_تهران_پاسداران_دیوار/gYB3nfvR</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>آپارتمان  دونبش و نورگیر عالی و شمالی
-دسترسی عالی به مترو و اتوبوس و خبابان اصلی
-پارکینگ غیرمزاحم
-بازدید= خرید
-جعفری : ۰۹۱۲۵۰۸۱۲۵۸</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>۱۴۰۰</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>۲</t>
-        </is>
-      </c>
+          <t>بایلام خدمت شما دوستان عزیز اجاره واحد تک خواب با پارکینگ سرپوشیده وساختمان ساکت و دنج فول امکانات دسترسی سریع و راحت به مراکز خرید رستوران فست فود و دسترسی سریع به بزرگراها 
+دسترسی ده دقیقه ای تا نمایشگاه بین المللی 
+لطفا جهت هماهنگی ورزرو بامادر ارتباط باشید باتشکر</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>۹۰</t>
+          <t>۷۰</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>انباری ندارد</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>قیمت کلتوافقی</t>
-        </is>
-      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره کوتاه مدت</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>آپارتمان و سوئیت</t>
         </is>
       </c>
       <c r="S17" t="inlineStr"/>
@@ -1846,75 +1840,59 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>دفترکار کاملا فرنیش با کلیه امکانات</t>
+          <t>زمین ۱۹۵ متری واقع در نیاوران خیابان بوکان</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ودیعه: ۱,۰۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۲۵,۰۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ر   و ن ک</t>
+          <t>نیاوران</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/دفترکار-کاملا-فرنیش-با-کلیه-امکانات_دفتر-کار-اتاق-اداری-و-مطب_تهران_ونک_دیوار/gYBXZsHI</t>
+          <t>https://divar.ir/v/زمین-۱۹۵-متری-واقع-در-نیاوران-خیابان-بوکان_زمین-و-کلنگی_تهران_نیاوران_دیوار/gYBbqbSi</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>دفتر کار کاملا فرنیش با کلیه امکانات</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>۱۳۹۶</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>۴</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>۱۴۰</t>
-        </is>
-      </c>
+          <t>این زمین ۱۹۵ متری از زمین های مهاب قدس فعلا در حال حاظر مجوز ساخت ندارد. سند منگوله دار دارد. نقشه هوایی دارد. طرح تفصیلی هم دارد. بهترین زمان و لحظه برای مبدل ساختن سرمایه‌گذاری کوتاه مدت به بلند مدت  زمینی ارزشمند و گرانبها است به دلیل نیاز مالی فروش فوری فوری فوری من فروشنده واقعی هستم فقط خریدار واقعی لطفا تماس بگیرید</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>آسانسور ندارد</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۱۲۸٬۲۰۵٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>قیمت کل۲۵٬۰۰۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>اجاره اداری و تجاری</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>دفتر کار، اتاق اداری و مطب</t>
+          <t>زمین و کلنگی</t>
         </is>
       </c>
       <c r="S18" t="inlineStr"/>
@@ -1925,81 +1903,74 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>اپارتمان ۷۵متری فرجام غربی</t>
+          <t>نوساز شیک 57 متر عروس دامادی</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ودیعه: ۵۳۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۱,۰۵۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ر   ت ه ر ا ن پ ا ر س   غ ر ب ی</t>
+          <t>بریانک</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/اپارتمان-۷۵متری-فرجام-غربی_آپارتمان_تهران_تهرانپارس-غربی_دیوار/gYBXJziK</t>
+          <t>https://divar.ir/v/نوساز-شیک-57-متر-عروس-دامادی_زمین-و-کلنگی_تهران_بریانک_دیوار/gYBXaK4u</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>تخلیه
-قابل تبدیل
-املاک تماس نگیرد لطفا</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>۱۳۹۱</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>۱</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>۷۵</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>طبقه۴ از ۵</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+          <t>ملک واقع در خیابان مولوی 
+یک خواب بزرگ و مستر
+سند تک برگ و اماده انتقال 
+سالن بزرگ و چهارگوش مناسب هر چیدمان 
+کابینت mdf، پکیج و رادیاتور .. فول امکانات و شیک
+مشاعات تمام سنگ کاری شده و تمیز .. همسایه ها عالی 
+دو عدد کولر گازی 
+فول امکانات،پارکینگ ،آسانسور ،تراس 
+واحد جنوبی رو به آفتاب با نورگیری فوق العاده 
+گذر پهن و عالی 
+دوربین مدار بسته
+دسترسی عالی به دو مترو میدان محمدیه و مولوی با شش دقیقه پیاده روی 
+بهترین لوکیشن منطقه 
+150تومان و ماهی 500 در رهن مستاجر که از مبلغ کل کم می شود .
+⛔فوری فوری فوری به دلیل بدهی 
+فروشنده واقعی</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>قیمت هر متر۱۸٬۴۲۱٬۰۰۰ تومان</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>قیمت کل۱٬۰۵۰٬۰۰۰٬۰۰۰ تومان</t>
+        </is>
+      </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>زمین و کلنگی</t>
         </is>
       </c>
       <c r="S19" t="inlineStr"/>
@@ -2010,68 +1981,45 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>۵۷ متر خوش نقشه یکخواب نور گیر  سند تک برگ</t>
+          <t>زمین مهراباد</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>۱,۵۵۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۴,۹۷۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ر   خ و ا ج ه   ن ص ی ر   ط و س ی</t>
+          <t>نارمک</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/۵۷-متر-خوش-نقشه-یکخواب-نور-گیر-سند-تک-برگ_آپارتمان_تهران_خواجه-نصیر-طوسی_دیوار/gYBPZWM9</t>
+          <t>https://divar.ir/v/زمین-مهراباد_زمین-و-کلنگی_تهران_نارمک_دیوار/gYBPq11O</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>۵۷ متر زیر همکف نور گیر عالی کوچه دنج و ارام . همسایگان خوب شوفاژ مرکزی کولر ابی کابینت فلز</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>۱۳۷۳</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>۱</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>۵۷</t>
-        </is>
-      </c>
+          <t>یک قطعه زمین با مساحت 482 متر مربع.دارای ویو فوق العاده.انشعابات آب و برق و گاز تا جلوی درب. خیابان آسفالت.سند وکالتی.موقعیت عالی.بسیار نزدیک جاده
+موقعیت:رودهن،مهراباد،گلزار محمد ابتدای کوچه طالبی</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>پارکینگ ندارد</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>آسانسور ندارد</t>
-        </is>
-      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
-          <t>قیمت هر متر۲۷٬۱۹۲٬۰۰۰ تومان</t>
+          <t>قیمت هر متر۱۰٬۳۱۱٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>قیمت کل۱٬۵۵۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کل۴٬۹۷۰٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2086,7 +2034,7 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>زمین و کلنگی</t>
         </is>
       </c>
       <c r="S20" t="inlineStr"/>
@@ -2097,58 +2045,46 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>۱۷۰متر نوساز تکواحدی فردوس شرق۲پارکینگ</t>
+          <t>٨٣ متر ١ خواب</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>۹,۱۸۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۴۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ر   ک و ی   ف ر د و س</t>
+          <t>جمهوری</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/۱۷۰متر-نوساز-تکواحدی-فردوس-شرق۲پارکینگ_آپارتمان_تهران_کوی-فردوس_دیوار/gY3NMTCj</t>
+          <t>https://divar.ir/v/٨٣-متر-١-خواب_آپارتمان_تهران_جمهوری_دیوار/gY_i_rlX</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>سرمایه گذاران و خریداران واقعی بشتابید
-۱میلیارد زیر قیمت منطقه
-۱۷۰متر
-بلوار فردوس شرق
-تکواحدی
-۲پارکینگ سندی
-نوساز
-تخلیه
-سند آماده
-روف گاردن
-رو به افتاب
-مالک فروشنده واقعی
-بازدید=خرید
-املاک.        (سهیل.   ۰۹۱۲۲۸۹۰۴۹۱</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>۱۴۰۰</t>
-        </is>
-      </c>
+          <t>٨٣ متر ١ خواب واقع در میدان جمهوری نبش ارومیه ی شرقی دسترسی راحت به مترو و بی آرتی 
+مناسب برای سکونت و دفتر کار</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>۳</t>
+          <t>۱</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>۱۷۰</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
+          <t>۸۳</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>طبقه۱ از ۳</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -2161,27 +2097,19 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۵۴٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>قیمت کل۹٬۱۸۰٬۰۰۰٬۰۰۰ تومان</t>
-        </is>
-      </c>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>فروش مسکونی</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2197,45 +2125,69 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>۸۷ و نیم متری پرنور و ضد زلزله</t>
+          <t>149متر 3خوابه سالن L طبقه پنجم ویو گلستان</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>۲,۹۵۰,۰۰۰,۰۰۰ تومان</t>
+          <t>۲۱,۶۰۵,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ر   ت ه ر ا ن ‌ س ر</t>
+          <t>پاسداران</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/۸۷-و-نیم-متری-پرنور-و-ضد-زلزله_آپارتمان_تهران_تهران-سر_دیوار/gY0Q5mTX</t>
+          <t>https://divar.ir/v/149متر-3خوابه-سالن-l-طبقه-پنجم-ویو-گلستان_آپارتمان_تهران_پاسداران_دیوار/gYBfKQGT</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>فول امکانات زندگی و دارای امتیازات فراوان و دو ورودی و چهار آسانسور و امکانات و دسترسی عالی به متروی اکباتان و متروی بیمه ومتروی  آزادی و بازارهای و مراکز خریدو پارک های  فراوان در اطراف 
-انباری بالای ملک و پارکینگ در طبقه همکف و بالکن ۷ متر ی ومنزل  بازسازی شده
- خودم مالک هستم ۰۹۰۳۰۷۵۸۵۰۳ لطفا
- املاکی در صورت آوردن مشتری تماس بگیرد۰</t>
+          <t>سعید نوری هستم 
+کارشناس فروش 3 خواب در پاسداران و دروس
+__________________________________________
+املاک بزرگ ایوان  **VIP**  همراه همیشگی شما
+__________________________________________
+⚜️ ⚜️ همان چیزی که در ذهن شماست ⚜️ ⚜️
+   #فروش فوری 
+️لوکیشن دنج و ایده آل واقع در گلستان✔️
+▫️ورودی باشکوه از لابی ارتفاع سقف بلند✔️
+️149متر 3 خواب یک خواب مستر ✔️
+▫️پلان کاربردی L سالن بزرگ و پر نور  ✔️
+️اتاق ها استاندارد کمد دیواری فراوان✔️
+▫️آشپزخانه بزرگ و پر کابینت های گلاس ✔️
+    و ...
+️مناسب سخت پسندان و مشگل پسندان✔️
+▫️به علت منحصر بودن فایل از گذاشتن عکسهای 
+واحد معذوریم ✔️
+️قیمت توافقی است 
+⚜️⚜️ انتخاب بر اساس توان شما و هنر ما ⚜️⚜️
+__________________________________________
+مشاور شما :  سعید نوری 
+شماره تماس : 09125721373 
+جهت اطلاعات بیشتر و هماهنگی جهت بازدید 
+با من تماس بگیرید . سپاس 
+__________________________________________
+▫️پیشنهاد میکنم قبل از تصمیم به خرید در منطقه 
+▫️حتما از این مورد هم دیدن کنید ✔️✔️✔️
+⭕ ⭕  پاسخ‌گویی از ساعت 8 الی 23  ⭕ ⭕</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>۱۳۹۴</t>
+          <t>۱۴۰۰</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۳</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>۸۸</t>
+          <t>۱۴۹</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -2256,12 +2208,12 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>قیمت هر متر۳۳٬۵۲۲٬۰۰۰ تومان</t>
+          <t>قیمت هر متر۱۴۵٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>قیمت کل۲٬۹۵۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کل۲۱٬۶۰۵٬۰۰۰٬۰۰۰ تومان</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2287,83 +2239,43 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>آپارتمان فول امکانات ، ۷۹ متری ،۲ خواب</t>
+          <t>زمین مسکونی</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>۳,۳۵۰,۰۰۰,۰۰۰ تومان</t>
+          <t>توافقی</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ر   آ ش ت ی ا ن ی</t>
+          <t>نازی‌آباد</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-فول-امکانات-۷۹-متری-۲-خواب_آپارتمان_تهران_آشتیانی_دیوار/gYBTJ3gm</t>
+          <t>https://divar.ir/v/زمین-مسکونی_زمین-و-کلنگی_تهران_نازی-آباد_دیوار/gYBf63bm</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>۷۹ متر سندی، ۱۲ متر پاسیو بازسازی شده که به ۷۹ متر اضافه می‌گردد(رویت ۹۵ متری)
-پاسیو مسقف( کف پارکت ، دیوار کوب طرح چوب ، ۲ تا پنجره روی سقف جهت تبادل هوا )
-کل واحد بازسازی شده
-متریال ساختمان بسیار عالی
-کف کل واحد سنگ درجه یک (پذیرایی،خواب‌هاوآشپزخانه)
-اتاق خواب بزرگ و جادار ( تخت خواب ۲نفره خور )
-کاغذ دیواری ایتالیایی
-آشپزخانه جادار و قابل گذاشتن میز نهار خوری ( مورد پسند خانم‌های خانه )
-سرایدار مستقر و ۲۴ ساعته
-پارکینگ قابل پارک ۲ ماشین
-مجتمع کم جمعیت و ساکت با همسایه های موجه
-دسترسی راحت به مراکز خرید، بانک، خیابان اصلی و اتوبان
-مشاعات دلپذیر و جذاب که تازه رنگ شده
-نور از پاسیو میگیرد
-لطفاً خریدار واقعی تماس بگیرد
-قیمت مقطوع</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>۱۳۸۶</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>۲</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>۷۹</t>
-        </is>
-      </c>
+          <t>زمین مسکونی واقع در کهریزک سند تک برگ
+فوری فروشی زیر قیمت منطقه
+لطفا با این شماره تماس بگیرید&gt;09191362037
+09191362037</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>انباری</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>پارکینگ</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>آسانسور</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>قیمت هر متر۴۲٬۴۰۵٬۰۰۰ تومان</t>
-        </is>
-      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
-          <t>قیمت کل۳٬۳۵۰٬۰۰۰٬۰۰۰ تومان</t>
+          <t>قیمت کلتوافقی</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2378,7 +2290,7 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>زمین و کلنگی</t>
         </is>
       </c>
       <c r="S23" t="inlineStr"/>
@@ -2389,59 +2301,45 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>آپارتمان ۱۱۰متر تک واحدی ۲خواب</t>
+          <t>خانه ویلایی ۱۱۵ متری</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ودیعه: ۵۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>توافقی</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ر   ا و ق ا ف</t>
+          <t>پونک</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/آپارتمان-۱۱۰متر-تک-واحدی-۲خواب_آپارتمان_تهران_اوقاف_دیوار/gYBXpHZJ</t>
+          <t>https://divar.ir/v/خانه-ویلایی-۱۱۵-متری_خانه-و-ویلا_تهران_پونک_دیوار/gYBfa2oS</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>طبقه روی همکف دوطرفه نورگیر گاز تو کار، فرتو کار، هود لمسی کابینت ام دی اف
-یک خواب مستر 
-هر دو اتاق کمد دیواری 
-یکی از اتاق ها ۱۵متر 
-یکی ۱۲متر 
-انباری ۹متر 
-بالکن روبه حیاط 
-ملک جنوبی
-دوخط تلفن 
-اینترنت وای فای فعال
-لطفا مشاوره املاک تماس نگیرد فقط مصرف کننده</t>
+          <t>خانه ای با زمین ۱۱۵ متر در دو طبقه ۷۰ متری قابل سکونت با فضای سبز بسیار عالی و دنج در محله پونک</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>۱۳۷۶</t>
+          <t>۱۳۷۹</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>۲</t>
+          <t>۳</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>۱۱۰</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>طبقه۱ از ۳</t>
-        </is>
-      </c>
+          <t>۱۴۰</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
           <t>انباری</t>
@@ -2449,29 +2347,25 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>پارکینگ ندارد</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>آسانسور ندارد</t>
-        </is>
-      </c>
+          <t>پارکینگ</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>اجاره مسکونی</t>
+          <t>فروش مسکونی</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>آپارتمان</t>
+          <t>خانه و ویلا</t>
         </is>
       </c>
       <c r="S24" t="inlineStr"/>
@@ -2482,44 +2376,65 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>مغازه ده متر نزدیک به بیست متری</t>
+          <t>اجاره اپارتمان</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ودیعه: ۱۰۰,۰۰۰,۰۰۰ تومان</t>
+          <t>ودیعه: ۶۰۰,۰۰۰,۰۰۰ تومان</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ر   ا ف س ر ی ه</t>
+          <t>ونک</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://divar.ir/v/مغازه-ده-متر-نزدیک-به-بیست-متری_مغازه-و-غرفه_تهران_افسریه_دیوار/gYBXZjZs</t>
+          <t>https://divar.ir/v/اجاره-اپارتمان_آپارتمان_تهران_ونک_دیوار/gYBb6UVO</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>مغازه ده متری نزدیک به بیست متری پانزده متری دوم</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
+          <t>جاره آپارتمان یک واحد از دو واحد سه خوابه رهن600  میلیون اجاره15میلیون شیخ بهایى امداد غربى
+09121445686</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>۱۳۷۵</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>+۴</t>
+          <t>۳</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>۱۰</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+          <t>۱۵۵</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>طبقههمکف</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>انباری</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>پارکینگ</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>آسانسور ندارد</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
@@ -2529,12 +2444,12 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>اجاره اداری و تجاری</t>
+          <t>اجاره مسکونی</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>مغازه و غرفه</t>
+          <t>آپارتمان</t>
         </is>
       </c>
       <c r="S25" t="inlineStr"/>

</xml_diff>